<commit_message>
change nasi to others
</commit_message>
<xml_diff>
--- a/Data/Sprint 1/Data Clara.xlsx
+++ b/Data/Sprint 1/Data Clara.xlsx
@@ -5302,7 +5302,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5892,8 +5892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O725"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A714" workbookViewId="0">
-      <selection activeCell="B727" sqref="B727"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6683,7 +6683,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>1524</v>
+        <v>4</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>1501</v>
@@ -6713,7 +6713,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>1524</v>
+        <v>4</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>1501</v>
@@ -7133,7 +7133,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>1524</v>
+        <v>4</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>1501</v>
@@ -7163,7 +7163,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>1524</v>
+        <v>4</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>1501</v>
@@ -11813,7 +11813,7 @@
         <v>1</v>
       </c>
       <c r="F190" s="2" t="s">
-        <v>1524</v>
+        <v>4</v>
       </c>
       <c r="G190" s="2" t="s">
         <v>1501</v>
@@ -11843,7 +11843,7 @@
         <v>1</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>1524</v>
+        <v>4</v>
       </c>
       <c r="G191" s="2" t="s">
         <v>1501</v>
@@ -13329,7 +13329,7 @@
         <v>1</v>
       </c>
       <c r="F240" s="2" t="s">
-        <v>1524</v>
+        <v>4</v>
       </c>
       <c r="G240" s="2" t="s">
         <v>1501</v>

</xml_diff>